<commit_message>
changed to a different directory
</commit_message>
<xml_diff>
--- a/app/framework/framework.xlsx
+++ b/app/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="1920" windowWidth="27380" windowHeight="17120" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1680" yWindow="0" windowWidth="25820" windowHeight="16220" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="87">
   <si>
     <t>comments</t>
   </si>
@@ -250,6 +250,39 @@
   </si>
   <si>
     <t>Plot</t>
+  </si>
+  <si>
+    <t>geotagger</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/geotagger/forms/geotagger/',null)</t>
+  </si>
+  <si>
+    <t>Geotagger</t>
+  </si>
+  <si>
+    <t>geoweather</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/geoweather/forms/geoweather/',null)</t>
+  </si>
+  <si>
+    <t>agriculture</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/agriculture/forms/agriculture/',null)</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>send_sms</t>
+  </si>
+  <si>
+    <t>Send SMS</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../tables/send_sms/forms/send_sms/',null)</t>
   </si>
 </sst>
 </file>
@@ -297,8 +330,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +426,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -418,6 +461,11 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -452,6 +500,11 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,10 +841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -881,14 +934,14 @@
     </row>
     <row r="8" spans="1:9" ht="17" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="59" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
@@ -904,16 +957,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.5" customHeight="1">
+    <row r="11" spans="1:9" ht="17" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="59" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -929,16 +982,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.5" customHeight="1">
+    <row r="14" spans="1:9" ht="17" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="66" customHeight="1">
+    <row r="15" spans="1:9" ht="59" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -955,14 +1008,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="66" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="59" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -979,14 +1033,15 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.5" customHeight="1">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -1004,13 +1059,13 @@
     </row>
     <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
         <v>41</v>
@@ -1028,13 +1083,13 @@
     </row>
     <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
         <v>41</v>
@@ -1052,13 +1107,13 @@
     </row>
     <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1076,13 +1131,13 @@
     </row>
     <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E33" t="s">
         <v>41</v>
@@ -1100,13 +1155,13 @@
     </row>
     <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
         <v>41</v>
@@ -1124,13 +1179,13 @@
     </row>
     <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
         <v>41</v>
@@ -1148,13 +1203,13 @@
     </row>
     <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1172,13 +1227,13 @@
     </row>
     <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
@@ -1196,13 +1251,13 @@
     </row>
     <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E48" t="s">
         <v>41</v>
@@ -1220,13 +1275,13 @@
     </row>
     <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E51" t="s">
         <v>41</v>
@@ -1244,13 +1299,13 @@
     </row>
     <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E54" t="s">
         <v>41</v>
@@ -1268,13 +1323,13 @@
     </row>
     <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E57" t="s">
         <v>41</v>
@@ -1287,6 +1342,102 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="66" customHeight="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17" customHeight="1">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="66" customHeight="1">
+      <c r="A63" s="3"/>
+      <c r="B63" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" t="s">
+        <v>41</v>
+      </c>
+      <c r="G63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17" customHeight="1">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="66" customHeight="1">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>41</v>
+      </c>
+      <c r="G66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="17" customHeight="1">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17.5" customHeight="1">
+      <c r="A68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="66" customHeight="1">
+      <c r="A69" s="3"/>
+      <c r="B69" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E69" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17" customHeight="1">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1437,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1465,11 +1616,11 @@
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1477,10 +1628,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1488,21 +1639,21 @@
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1510,10 +1661,10 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1521,10 +1672,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1532,10 +1683,10 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1543,10 +1694,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1554,10 +1705,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1565,10 +1716,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1576,10 +1727,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1587,10 +1738,10 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1598,10 +1749,10 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1609,10 +1760,10 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1620,10 +1771,10 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1631,10 +1782,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1642,10 +1793,54 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>